<commit_message>
add US to AHDI table
</commit_message>
<xml_diff>
--- a/data/albco_profile_raceovertime.xlsx
+++ b/data/albco_profile_raceovertime.xlsx
@@ -1,33 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/micheleclaibourn/Box Sync/mpc/dataForDemocracy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mpc8t/Box Sync/mpc/dataForDemocracy/albequity_profile/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C266D679-0357-8E4E-A49D-B4F9B926FE50}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB052729-1DDE-E447-8547-F9926FB4A511}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1180" yWindow="1460" windowWidth="27240" windowHeight="15000" xr2:uid="{6563C26B-1A75-1D41-85EE-45A2BEFE4257}"/>
+    <workbookView xWindow="1180" yWindow="1400" windowWidth="27240" windowHeight="15000" xr2:uid="{6563C26B-1A75-1D41-85EE-45A2BEFE4257}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="2" r:id="rId1"/>
     <sheet name="social_exp" sheetId="1" r:id="rId2"/>
     <sheet name="sources" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="66">
   <si>
     <t>Total Population:</t>
   </si>
@@ -222,6 +231,9 @@
   </si>
   <si>
     <t>nonwhite_per</t>
+  </si>
+  <si>
+    <t>2019 ACS 1</t>
   </si>
 </sst>
 </file>
@@ -295,7 +307,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -310,19 +322,13 @@
     <xf numFmtId="3" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
@@ -640,10 +646,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A89E56FA-C5D2-2341-A90C-957738BC42D4}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -718,11 +724,11 @@
         <v>7643</v>
       </c>
       <c r="F3" s="5">
-        <f t="shared" ref="F3:F24" si="0">(D3/C3)*100</f>
+        <f t="shared" ref="F3:F25" si="0">(D3/C3)*100</f>
         <v>53.506904312914415</v>
       </c>
       <c r="G3" s="5">
-        <f t="shared" ref="G3:G24" si="1">100-F3</f>
+        <f t="shared" ref="G3:G25" si="1">100-F3</f>
         <v>46.493095687085585</v>
       </c>
     </row>
@@ -1249,6 +1255,31 @@
       <c r="G24" s="5">
         <f t="shared" si="1"/>
         <v>19.432151156916234</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
+        <v>2019</v>
+      </c>
+      <c r="B25" s="12">
+        <v>109722</v>
+      </c>
+      <c r="C25" s="6">
+        <v>109330</v>
+      </c>
+      <c r="D25" s="6">
+        <v>89592</v>
+      </c>
+      <c r="E25" s="6">
+        <v>19738</v>
+      </c>
+      <c r="F25" s="5">
+        <f t="shared" si="0"/>
+        <v>81.946400804902581</v>
+      </c>
+      <c r="G25" s="5">
+        <f t="shared" si="1"/>
+        <v>18.053599195097419</v>
       </c>
     </row>
   </sheetData>
@@ -1263,13 +1294,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B23CA8-6B4B-5445-9266-3D62A0441AB1}">
-  <dimension ref="A1:E134"/>
+  <dimension ref="A1:E144"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B127" sqref="B127:B128"/>
+    <sheetView topLeftCell="A125" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D138" sqref="D138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1">
@@ -2546,6 +2580,107 @@
       <c r="D134" s="1">
         <f>SUM(B129:B134)</f>
         <v>19232</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A137" t="s">
+        <v>43</v>
+      </c>
+      <c r="B137" s="1">
+        <v>109330</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>44</v>
+      </c>
+      <c r="B138" s="1">
+        <v>89592</v>
+      </c>
+      <c r="C138" s="2">
+        <f>B138/$B$137</f>
+        <v>0.81946400804902586</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>45</v>
+      </c>
+      <c r="B139" s="1">
+        <v>9954</v>
+      </c>
+      <c r="C139" s="2">
+        <f t="shared" ref="C139:C144" si="0">B139/$B$137</f>
+        <v>9.1045458703009244E-2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>46</v>
+      </c>
+      <c r="B140">
+        <v>266</v>
+      </c>
+      <c r="C140" s="2">
+        <f t="shared" si="0"/>
+        <v>2.4330010061282357E-3</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>47</v>
+      </c>
+      <c r="B141" s="1">
+        <v>5462</v>
+      </c>
+      <c r="C141" s="2">
+        <f t="shared" si="0"/>
+        <v>4.9958840208542944E-2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>48</v>
+      </c>
+      <c r="B142">
+        <v>115</v>
+      </c>
+      <c r="C142" s="2">
+        <f t="shared" si="0"/>
+        <v>1.0518613372358914E-3</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>49</v>
+      </c>
+      <c r="B143" s="1">
+        <v>519</v>
+      </c>
+      <c r="C143" s="2">
+        <f t="shared" si="0"/>
+        <v>4.747095948047197E-3</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>50</v>
+      </c>
+      <c r="B144" s="1">
+        <v>3422</v>
+      </c>
+      <c r="C144" s="2">
+        <f t="shared" si="0"/>
+        <v>3.1299734748010608E-2</v>
+      </c>
+      <c r="D144" s="1">
+        <f>SUM(B139:B144)</f>
+        <v>19738</v>
       </c>
     </row>
   </sheetData>

</xml_diff>